<commit_message>
Add error-catching where data is missing
</commit_message>
<xml_diff>
--- a/Data/database_glossary.xlsx
+++ b/Data/database_glossary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterlehner/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterlehner/Library/CloudStorage/Dropbox/Climata_GoingSolo/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B23886B-0A17-9A42-95AA-6C9895F10B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40418F7A-2B56-4E41-BFF9-E0E556034C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-8320" windowWidth="21600" windowHeight="37900" xr2:uid="{339229BC-2F47-AB4F-8453-12FE96792110}"/>
+    <workbookView xWindow="38400" yWindow="-8320" windowWidth="21600" windowHeight="18940" xr2:uid="{339229BC-2F47-AB4F-8453-12FE96792110}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -174,10 +174,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -228,6 +235,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,509 +556,522 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D12016CC-2245-564F-9745-C6E5A349F6EF}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="B2:G36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="215" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
         <v>2801</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D2" s="1">
         <v>2802</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E2" s="1">
         <v>2804</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C3" s="1">
         <v>41.530099999999997</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D3" s="1">
         <v>41.9512</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E3" s="1">
         <v>41.423099999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C4" s="1">
         <v>-71.284099999999995</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D4" s="1">
         <v>-71.454499999999996</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E4" s="1">
         <v>-71.783699999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C7" s="1">
         <v>7074</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D7" s="1">
         <v>7074</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E7" s="1">
         <v>7074</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="C9" s="1">
         <v>0.168462424</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D9" s="1">
         <v>0.168462424</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E9" s="1">
         <v>0.168462424</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="G9">
+        <f>28296/20</f>
+        <v>1414.8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C10" s="1">
         <v>0.2223704</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D10" s="1">
         <v>0.2223704</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E10" s="1">
         <v>0.2223704</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="G10" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="5">
+      <c r="C11" s="5">
         <v>131</v>
       </c>
-      <c r="C10" s="5">
+      <c r="D11" s="5">
         <v>131</v>
       </c>
-      <c r="D10" s="5">
+      <c r="E11" s="5">
         <v>131</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="G11">
+        <f>G9/G10</f>
+        <v>0.28295999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="1">
+      <c r="C13" s="1">
         <v>16.18</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D13" s="1">
         <v>16.18</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E13" s="1">
         <v>16.18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="1">
+      <c r="C15" s="1">
         <v>1410</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D15" s="1">
         <v>1322</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E15" s="1">
         <v>1361</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="1">
+      <c r="C16" s="1">
         <v>7.0921985815602842E-4</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D16" s="1">
         <v>7.5642965204236008E-4</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E16" s="1">
         <v>7.347538574577516E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="1">
+      <c r="C17" s="1">
         <v>0.16095890410958905</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D17" s="1">
         <v>0.15091324200913242</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E17" s="1">
         <v>0.15536529680365296</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D18" s="1">
         <v>1207</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E18" s="1">
         <v>1602</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="1">
+      <c r="C19" s="1">
         <v>1751</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D19" s="1">
         <v>1751</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E19" s="1">
         <v>1751</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="1">
+      <c r="C20" s="1">
         <v>1701</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D20" s="1">
         <v>1701</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E20" s="1">
         <v>1701</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
+      <c r="C22" s="1">
         <v>3440</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D22" s="1">
         <v>3440</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E22" s="1">
         <v>3440</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="1">
+      <c r="C23" s="1">
         <v>417</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D23" s="1">
         <v>482</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E23" s="1">
         <v>501</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="1">
+      <c r="C24" s="1">
         <v>967</v>
       </c>
-      <c r="C23" s="1">
+      <c r="D24" s="1">
         <v>845</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E24" s="1">
         <v>915</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="1">
+      <c r="C25" s="1">
         <v>7159</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D25" s="1">
         <v>6600</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E25" s="1">
         <v>6901</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="1">
-        <f>ROUND(B22*B9+B23*B12/10,0)</f>
+      <c r="C26" s="1">
+        <f>ROUND(C23*C10+C24*C13/10,0)</f>
         <v>1657</v>
       </c>
-      <c r="C25" s="1">
-        <f>ROUND(C22*C9+C23*C12/10,0)</f>
+      <c r="D26" s="1">
+        <f>ROUND(D23*D10+D24*D13/10,0)</f>
         <v>1474</v>
       </c>
-      <c r="D25" s="1">
-        <f>ROUND(D22*D9+D23*D12/10,0)</f>
+      <c r="E26" s="1">
+        <f>ROUND(E23*E10+E24*E13/10,0)</f>
         <v>1592</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="1">
-        <f>ROUND(B24*B9,0)</f>
+      <c r="C27" s="1">
+        <f>ROUND(C25*C10,0)</f>
         <v>1592</v>
       </c>
-      <c r="C26" s="1">
-        <f>ROUND(C24*C9,0)</f>
+      <c r="D27" s="1">
+        <f>ROUND(D25*D10,0)</f>
         <v>1468</v>
       </c>
-      <c r="D26" s="1">
-        <f>ROUND(D24*D9,0)</f>
+      <c r="E27" s="1">
+        <f>ROUND(E25*E10,0)</f>
         <v>1535</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="1">
-        <f>B25-B26</f>
+      <c r="C28" s="1">
+        <f>C26-C27</f>
         <v>65</v>
       </c>
-      <c r="C27" s="1">
-        <f>C25-C26</f>
+      <c r="D28" s="1">
+        <f>D26-D27</f>
         <v>6</v>
       </c>
-      <c r="D27" s="1">
-        <f>D25-D26</f>
+      <c r="E28" s="1">
+        <f>E26-E27</f>
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="1">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="1">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="1">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="1">
-        <v>0</v>
-      </c>
-      <c r="C32" s="1">
-        <v>0</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="1">
-        <v>0</v>
-      </c>
-      <c r="C33" s="1">
-        <v>0</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="1">
-        <v>0</v>
-      </c>
-      <c r="C34" s="1">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="1">
+      <c r="C36" s="1">
         <v>1</v>
       </c>
-      <c r="C35" s="1">
+      <c r="D36" s="1">
         <v>1</v>
       </c>
-      <c r="D35" s="1">
+      <c r="E36" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>